<commit_message>
fix some typo/bugs and add some explanation
</commit_message>
<xml_diff>
--- a/Doc/Timer_logic_timing_diagram.xlsx
+++ b/Doc/Timer_logic_timing_diagram.xlsx
@@ -272,17 +272,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AJ18" sqref="AJ18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AJ36" sqref="AJ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1081,7 +1081,7 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="10"/>
+      <c r="AA6" s="8"/>
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
@@ -1105,8 +1105,8 @@
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1133,8 +1133,8 @@
       <c r="AI8" s="4"/>
       <c r="AJ8" s="5"/>
       <c r="AK8" s="1"/>
-      <c r="AL8" s="9"/>
-      <c r="AM8" s="10"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="8"/>
       <c r="AN8" s="4"/>
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
@@ -1143,43 +1143,43 @@
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="7">
+      <c r="J10" s="10"/>
+      <c r="K10" s="9">
         <v>0</v>
       </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="7">
+      <c r="L10" s="10"/>
+      <c r="M10" s="9">
         <v>1</v>
       </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="7">
+      <c r="N10" s="10"/>
+      <c r="O10" s="9">
         <v>2</v>
       </c>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="7">
+      <c r="P10" s="10"/>
+      <c r="Q10" s="9">
         <v>3</v>
       </c>
-      <c r="R10" s="8"/>
-      <c r="S10" s="7">
+      <c r="R10" s="10"/>
+      <c r="S10" s="9">
         <v>4</v>
       </c>
-      <c r="T10" s="8"/>
-      <c r="U10" s="7">
+      <c r="T10" s="10"/>
+      <c r="U10" s="9">
         <v>5</v>
       </c>
-      <c r="V10" s="8"/>
-      <c r="W10" s="7">
+      <c r="V10" s="10"/>
+      <c r="W10" s="9">
         <v>6</v>
       </c>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="7">
+      <c r="X10" s="10"/>
+      <c r="Y10" s="9">
         <v>7</v>
       </c>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="7">
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="9">
         <v>7</v>
       </c>
       <c r="AB10" s="11"/>
@@ -1192,15 +1192,15 @@
       <c r="AI10" s="11"/>
       <c r="AJ10" s="11"/>
       <c r="AK10" s="11"/>
-      <c r="AL10" s="8"/>
-      <c r="AM10" s="7">
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="9">
         <v>0</v>
       </c>
-      <c r="AN10" s="8"/>
-      <c r="AO10" s="7">
+      <c r="AN10" s="10"/>
+      <c r="AO10" s="9">
         <v>1</v>
       </c>
-      <c r="AP10" s="8"/>
+      <c r="AP10" s="10"/>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -1226,7 +1226,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="6"/>
-      <c r="AA12" s="10"/>
+      <c r="AA12" s="8"/>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
@@ -1274,8 +1274,8 @@
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
       <c r="AG14" s="6"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="10"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="8"/>
       <c r="AJ14" s="4"/>
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
@@ -1402,7 +1402,7 @@
       <c r="AV25" s="6"/>
       <c r="AW25" s="6"/>
       <c r="AX25" s="6"/>
-      <c r="AY25" s="10"/>
+      <c r="AY25" s="8"/>
       <c r="AZ25" s="4"/>
       <c r="BA25" s="4"/>
       <c r="BB25" s="4"/>
@@ -1418,8 +1418,8 @@
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="10"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="8"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -1475,8 +1475,8 @@
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="10"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="8"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -1490,10 +1490,10 @@
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="9"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
       <c r="AC29" s="4"/>
       <c r="AD29" s="4"/>
       <c r="AE29" s="4"/>
@@ -1506,10 +1506,10 @@
       <c r="AL29" s="4"/>
       <c r="AM29" s="4"/>
       <c r="AN29" s="4"/>
-      <c r="AO29" s="4"/>
-      <c r="AP29" s="5"/>
-      <c r="AQ29" s="1"/>
-      <c r="AR29" s="9"/>
+      <c r="AO29" s="1"/>
+      <c r="AP29" s="7"/>
+      <c r="AQ29" s="4"/>
+      <c r="AR29" s="4"/>
       <c r="AS29" s="4"/>
       <c r="AT29" s="4"/>
       <c r="AU29" s="4"/>
@@ -1529,91 +1529,91 @@
       <c r="B31" t="s">
         <v>2</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="7">
+      <c r="J31" s="10"/>
+      <c r="K31" s="9">
         <v>0</v>
       </c>
-      <c r="L31" s="8"/>
-      <c r="M31" s="7">
+      <c r="L31" s="10"/>
+      <c r="M31" s="9">
         <v>1</v>
       </c>
-      <c r="N31" s="8"/>
-      <c r="O31" s="7">
+      <c r="N31" s="10"/>
+      <c r="O31" s="9">
         <v>2</v>
       </c>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="7">
+      <c r="P31" s="10"/>
+      <c r="Q31" s="9">
         <v>3</v>
       </c>
-      <c r="R31" s="8"/>
-      <c r="S31" s="7">
+      <c r="R31" s="10"/>
+      <c r="S31" s="9">
         <v>4</v>
       </c>
-      <c r="T31" s="8"/>
-      <c r="U31" s="7">
+      <c r="T31" s="10"/>
+      <c r="U31" s="9">
         <v>5</v>
       </c>
-      <c r="V31" s="8"/>
-      <c r="W31" s="7">
+      <c r="V31" s="10"/>
+      <c r="W31" s="9">
         <v>6</v>
       </c>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="7">
+      <c r="X31" s="10"/>
+      <c r="Y31" s="9">
         <v>7</v>
       </c>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="7">
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="9">
         <v>0</v>
       </c>
-      <c r="AB31" s="8"/>
-      <c r="AC31" s="7">
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="9">
         <v>1</v>
       </c>
-      <c r="AD31" s="8"/>
-      <c r="AE31" s="7">
+      <c r="AD31" s="10"/>
+      <c r="AE31" s="9">
         <v>2</v>
       </c>
-      <c r="AF31" s="8"/>
-      <c r="AG31" s="7">
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="9">
         <v>3</v>
       </c>
-      <c r="AH31" s="8"/>
-      <c r="AI31" s="7">
+      <c r="AH31" s="10"/>
+      <c r="AI31" s="9">
         <v>4</v>
       </c>
-      <c r="AJ31" s="8"/>
-      <c r="AK31" s="7">
+      <c r="AJ31" s="10"/>
+      <c r="AK31" s="9">
         <v>5</v>
       </c>
-      <c r="AL31" s="8"/>
-      <c r="AM31" s="7">
+      <c r="AL31" s="10"/>
+      <c r="AM31" s="9">
         <v>6</v>
       </c>
-      <c r="AN31" s="8"/>
-      <c r="AO31" s="7">
+      <c r="AN31" s="10"/>
+      <c r="AO31" s="9">
         <v>7</v>
       </c>
-      <c r="AP31" s="8"/>
-      <c r="AQ31" s="7">
+      <c r="AP31" s="10"/>
+      <c r="AQ31" s="9">
         <v>0</v>
       </c>
-      <c r="AR31" s="8"/>
-      <c r="AS31" s="7">
+      <c r="AR31" s="10"/>
+      <c r="AS31" s="9">
         <v>1</v>
       </c>
-      <c r="AT31" s="8"/>
-      <c r="AU31" s="7">
+      <c r="AT31" s="10"/>
+      <c r="AU31" s="9">
         <v>2</v>
       </c>
-      <c r="AV31" s="8"/>
-      <c r="AW31" s="7">
+      <c r="AV31" s="10"/>
+      <c r="AW31" s="9">
         <v>3</v>
       </c>
-      <c r="AX31" s="8"/>
-      <c r="AY31" s="7">
+      <c r="AX31" s="10"/>
+      <c r="AY31" s="9">
         <v>4</v>
       </c>
       <c r="AZ31" s="11"/>
@@ -1622,7 +1622,7 @@
       <c r="BC31" s="11"/>
       <c r="BD31" s="11"/>
       <c r="BE31" s="11"/>
-      <c r="BF31" s="8"/>
+      <c r="BF31" s="10"/>
     </row>
     <row r="33" spans="2:58" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
@@ -1648,7 +1648,7 @@
       <c r="X33" s="6"/>
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
-      <c r="AA33" s="10"/>
+      <c r="AA33" s="8"/>
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
       <c r="AD33" s="4"/>
@@ -1664,7 +1664,7 @@
       <c r="AN33" s="6"/>
       <c r="AO33" s="6"/>
       <c r="AP33" s="6"/>
-      <c r="AQ33" s="10"/>
+      <c r="AQ33" s="8"/>
       <c r="AR33" s="4"/>
       <c r="AS33" s="4"/>
       <c r="AT33" s="4"/>
@@ -1672,7 +1672,7 @@
       <c r="AV33" s="5"/>
       <c r="AW33" s="6"/>
       <c r="AX33" s="6"/>
-      <c r="AY33" s="10"/>
+      <c r="AY33" s="8"/>
       <c r="AZ33" s="4"/>
       <c r="BA33" s="4"/>
       <c r="BB33" s="4"/>
@@ -1683,20 +1683,14 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="AU31:AV31"/>
-    <mergeCell ref="AW31:AX31"/>
-    <mergeCell ref="AY31:BF31"/>
-    <mergeCell ref="AI31:AJ31"/>
-    <mergeCell ref="AK31:AL31"/>
-    <mergeCell ref="AM31:AN31"/>
-    <mergeCell ref="AO31:AP31"/>
-    <mergeCell ref="AQ31:AR31"/>
-    <mergeCell ref="AS31:AT31"/>
-    <mergeCell ref="W31:X31"/>
-    <mergeCell ref="Y31:Z31"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="AM10:AN10"/>
+    <mergeCell ref="AO10:AP10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
     <mergeCell ref="AG31:AH31"/>
     <mergeCell ref="AA10:AL10"/>
     <mergeCell ref="I31:J31"/>
@@ -1709,14 +1703,20 @@
     <mergeCell ref="U10:V10"/>
     <mergeCell ref="W10:X10"/>
     <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AM10:AN10"/>
-    <mergeCell ref="AO10:AP10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="W31:X31"/>
+    <mergeCell ref="Y31:Z31"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AE31:AF31"/>
+    <mergeCell ref="AU31:AV31"/>
+    <mergeCell ref="AW31:AX31"/>
+    <mergeCell ref="AY31:BF31"/>
+    <mergeCell ref="AI31:AJ31"/>
+    <mergeCell ref="AK31:AL31"/>
+    <mergeCell ref="AM31:AN31"/>
+    <mergeCell ref="AO31:AP31"/>
+    <mergeCell ref="AQ31:AR31"/>
+    <mergeCell ref="AS31:AT31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>